<commit_message>
N ew excel and add removing sum time
</commit_message>
<xml_diff>
--- a/count_time.xlsx
+++ b/count_time.xlsx
@@ -1,52 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Start_time</t>
-  </si>
-  <si>
-    <t>End_time</t>
-  </si>
-  <si>
-    <t>Work_time</t>
-  </si>
-  <si>
-    <t>Sum_time</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -65,19 +46,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -367,70 +410,297 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col width="17.140625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="13.28515625" customWidth="1" style="1" min="2" max="2"/>
+    <col width="15" customWidth="1" style="1" min="4" max="4"/>
+    <col width="12" bestFit="1" customWidth="1" style="1" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="D6"/>
-      <c r="E6"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Start_time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>End_time</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Work_time</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Sum_time</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>20:17:31</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20:17:38</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>00:00:07</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01:08:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>20:17:26</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>20:17:28</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>20:12:24</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>20:12:29</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>00:00:04</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>20:12:03</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>00:00:06</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>20:11:27</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20:11:47</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>00:00:20</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>15:16:16</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>15:26:35</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>00:10:18</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>15:05:33</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>15:16:04</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>00:10:30</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>14:18:27</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>15:05:20</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>00:46:52</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>14:10:03</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>14:10:07</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>00:00:04</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add desing and error com
</commit_message>
<xml_diff>
--- a/count_time.xlsx
+++ b/count_time.xlsx
@@ -415,10 +415,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E127"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="A2:E3"/>
+      <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -459,49 +459,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21:34:00</t>
+          <t>14:53:21</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>21:34:02</t>
+          <t>14:53:23</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>00:00:29</t>
+          <t>00:01:19</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21:33:57</t>
+          <t>14:53:17</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>21:33:59</t>
+          <t>14:53:19</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -513,22 +513,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>21:32:33</t>
+          <t>14:52:33</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>21:32:34</t>
+          <t>14:52:34</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -540,22 +540,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>21:32:31</t>
+          <t>14:51:07</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>21:32:31</t>
+          <t>14:51:25</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:18</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -567,17 +567,17 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>21:32:28</t>
+          <t>14:50:39</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>21:32:30</t>
+          <t>14:50:40</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -594,17 +594,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>21:32:26</t>
+          <t>14:50:36</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>21:32:27</t>
+          <t>14:50:37</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -621,22 +621,22 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>21:32:07</t>
+          <t>14:50:21</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>21:32:08</t>
+          <t>14:50:32</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:11</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -648,22 +648,22 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>21:32:05</t>
+          <t>14:45:35</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>21:32:06</t>
+          <t>14:45:36</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -675,17 +675,17 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>21:32:01</t>
+          <t>14:45:33</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>21:32:03</t>
+          <t>14:45:34</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -702,22 +702,22 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21:31:30</t>
+          <t>10:42:54</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>21:31:32</t>
+          <t>10:42:54</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -729,17 +729,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21:31:24</t>
+          <t>10:42:51</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>21:31:25</t>
+          <t>10:42:52</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -756,22 +756,22 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21:27:40</t>
+          <t>10:38:32</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>21:27:41</t>
+          <t>10:38:33</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -783,22 +783,22 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21:25:36</t>
+          <t>10:33:17</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>21:25:37</t>
+          <t>10:33:18</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -810,22 +810,22 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21:25:35</t>
+          <t>10:32:35</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>21:25:35</t>
+          <t>10:32:37</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -837,22 +837,22 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21:25:33</t>
+          <t>10:31:33</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>21:25:34</t>
+          <t>10:31:35</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -864,22 +864,22 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>21:23:50</t>
+          <t>10:29:44</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>21:24:00</t>
+          <t>10:29:45</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>00:00:09</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -891,17 +891,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>21:23:48</t>
+          <t>10:29:41</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>21:23:50</t>
+          <t>10:29:42</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -918,22 +918,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>21:23:46</t>
+          <t>10:11:12</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>21:23:46</t>
+          <t>10:11:13</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -945,22 +945,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>21:23:29</t>
+          <t>10:11:09</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>21:23:29</t>
+          <t>10:11:11</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -972,22 +972,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21:23:22</t>
+          <t>10:11:06</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>21:23:23</t>
+          <t>10:11:07</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -999,22 +999,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21:23:21</t>
+          <t>10:00:54</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>21:23:22</t>
+          <t>10:00:56</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1026,22 +1026,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21:23:08</t>
+          <t>10:00:49</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>21:23:09</t>
+          <t>10:00:52</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:03</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1053,22 +1053,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>21:23:02</t>
+          <t>10:00:45</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>21:23:02</t>
+          <t>10:00:47</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1080,22 +1080,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>21:21:47</t>
+          <t>10:00:42</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>21:21:48</t>
+          <t>10:00:43</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1107,22 +1107,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>21:21:46</t>
+          <t>10:00:36</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>21:21:46</t>
+          <t>10:00:38</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1134,17 +1134,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>21:21:43</t>
+          <t>09:59:40</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>21:21:45</t>
+          <t>09:59:41</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1161,22 +1161,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>21:21:25</t>
+          <t>09:59:37</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>21:21:25</t>
+          <t>09:59:39</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1188,17 +1188,17 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>21:21:23</t>
+          <t>09:59:22</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>21:21:23</t>
+          <t>09:59:22</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1215,17 +1215,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>21:21:20</t>
+          <t>09:59:18</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>21:21:21</t>
+          <t>09:59:18</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1242,22 +1242,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>21:21:01</t>
+          <t>09:59:14</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>21:21:01</t>
+          <t>09:59:16</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1269,22 +1269,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>21:20:59</t>
+          <t>09:58:45</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>21:21:00</t>
+          <t>09:58:47</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1296,17 +1296,17 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>21:20:57</t>
+          <t>09:58:40</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>21:20:58</t>
+          <t>09:58:42</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1323,17 +1323,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>21:20:55</t>
+          <t>09:55:57</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>21:20:56</t>
+          <t>09:55:57</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1350,22 +1350,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>21:16:55</t>
+          <t>09:55:55</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>21:16:57</t>
+          <t>09:55:56</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1377,22 +1377,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>21:16:53</t>
+          <t>09:55:53</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>21:16:54</t>
+          <t>09:55:54</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1404,22 +1404,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>21:16:49</t>
+          <t>09:55:24</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>21:16:50</t>
+          <t>09:55:27</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1431,22 +1431,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>21:10:35</t>
+          <t>09:54:52</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>21:10:35</t>
+          <t>09:54:57</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:04</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1458,22 +1458,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>21:10:15</t>
+          <t>09:54:50</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>21:10:16</t>
+          <t>09:54:52</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1485,17 +1485,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>21:10:14</t>
+          <t>09:52:50</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>21:10:15</t>
+          <t>09:52:51</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1512,22 +1512,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>21:10:12</t>
+          <t>09:52:45</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>21:10:13</t>
+          <t>09:52:47</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1539,22 +1539,22 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>21:08:54</t>
+          <t>09:52:42</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>21:08:54</t>
+          <t>09:52:44</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1566,22 +1566,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>21:08:51</t>
+          <t>09:52:39</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>21:08:52</t>
+          <t>09:52:40</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1593,22 +1593,22 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>21:08:49</t>
+          <t>09:52:10</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>21:08:51</t>
+          <t>09:52:11</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1620,22 +1620,22 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>21:08:46</t>
+          <t>09:52:08</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>21:08:49</t>
+          <t>09:52:09</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1647,17 +1647,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>21:07:20</t>
+          <t>09:52:07</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>21:07:20</t>
+          <t>09:52:08</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1674,22 +1674,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>21:07:14</t>
+          <t>09:52:05</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>21:07:15</t>
+          <t>09:52:06</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1701,22 +1701,22 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>26/09/2022</t>
+          <t>27/09/2022</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>21:03:01</t>
+          <t>09:52:01</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>21:03:03</t>
+          <t>09:52:03</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1733,66 +1733,66 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>21:02:53</t>
+          <t>21:34:00</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>21:02:56</t>
+          <t>21:34:02</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>00:00:29</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>23:34:10</t>
+          <t>21:33:57</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>23:34:10</t>
+          <t>21:33:59</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>00:00:33</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21:03:18</t>
+          <t>21:32:33</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>21:03:19</t>
+          <t>21:32:34</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1809,22 +1809,22 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>21:03:14</t>
+          <t>21:32:31</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>21:03:16</t>
+          <t>21:32:31</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1836,22 +1836,22 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>21:03:00</t>
+          <t>21:32:28</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>21:03:00</t>
+          <t>21:32:30</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1863,22 +1863,22 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>21:02:59</t>
+          <t>21:32:26</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>21:02:59</t>
+          <t>21:32:27</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1890,17 +1890,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>21:02:58</t>
+          <t>21:32:07</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>21:02:59</t>
+          <t>21:32:08</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1917,22 +1917,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>21:02:54</t>
+          <t>21:32:05</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>21:02:56</t>
+          <t>21:32:06</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1944,17 +1944,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>21:02:52</t>
+          <t>21:32:01</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>21:02:53</t>
+          <t>21:32:03</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1971,22 +1971,22 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>21:02:45</t>
+          <t>21:31:30</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>21:02:49</t>
+          <t>21:31:32</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>00:00:03</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1998,22 +1998,22 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>21:02:29</t>
+          <t>21:31:24</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>21:02:34</t>
+          <t>21:31:25</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2025,17 +2025,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>21:02:21</t>
+          <t>21:27:40</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>21:02:22</t>
+          <t>21:27:41</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2052,22 +2052,22 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>21:02:19</t>
+          <t>21:25:36</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>21:02:20</t>
+          <t>21:25:37</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2079,17 +2079,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>21:02:17</t>
+          <t>21:25:35</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>21:02:18</t>
+          <t>21:25:35</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -2106,17 +2106,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>21:00:56</t>
+          <t>21:25:33</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>21:00:57</t>
+          <t>21:25:34</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -2133,22 +2133,22 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>21:00:55</t>
+          <t>21:23:50</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>21:00:56</t>
+          <t>21:24:00</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:09</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2160,22 +2160,22 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>21:00:53</t>
+          <t>21:23:48</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>21:00:54</t>
+          <t>21:23:50</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2187,22 +2187,22 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>21:00:51</t>
+          <t>21:23:46</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>21:00:52</t>
+          <t>21:23:46</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2214,22 +2214,22 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>20:56:22</t>
+          <t>21:23:29</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>20:56:24</t>
+          <t>21:23:29</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2241,17 +2241,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>20:56:20</t>
+          <t>21:23:22</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>20:56:21</t>
+          <t>21:23:23</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2268,17 +2268,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>20:56:18</t>
+          <t>21:23:21</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>20:56:19</t>
+          <t>21:23:22</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2295,17 +2295,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>20:45:30</t>
+          <t>21:23:08</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>20:45:31</t>
+          <t>21:23:09</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2322,17 +2322,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>20:45:02</t>
+          <t>21:23:02</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>20:45:03</t>
+          <t>21:23:02</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -2349,22 +2349,22 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>20:40:53</t>
+          <t>21:21:47</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>20:40:54</t>
+          <t>21:21:48</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2376,17 +2376,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>20:40:00</t>
+          <t>21:21:46</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>20:40:01</t>
+          <t>21:21:46</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2403,17 +2403,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>20:34:57</t>
+          <t>21:21:43</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>20:34:58</t>
+          <t>21:21:45</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2430,17 +2430,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>20:32:57</t>
+          <t>21:21:25</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>20:32:57</t>
+          <t>21:21:25</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2457,22 +2457,22 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>20:32:54</t>
+          <t>21:21:23</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>20:32:55</t>
+          <t>21:21:23</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2484,22 +2484,22 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>20:32:50</t>
+          <t>21:21:20</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>20:32:52</t>
+          <t>21:21:21</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2511,17 +2511,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>20:31:27</t>
+          <t>21:21:01</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>20:31:28</t>
+          <t>21:21:01</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2538,17 +2538,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>20:30:38</t>
+          <t>21:20:59</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>20:30:39</t>
+          <t>21:21:00</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2565,22 +2565,22 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>20:22:47</t>
+          <t>21:20:57</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>20:22:50</t>
+          <t>21:20:58</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2592,17 +2592,17 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>20:22:45</t>
+          <t>21:20:55</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>20:22:46</t>
+          <t>21:20:56</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2619,17 +2619,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>20:22:43</t>
+          <t>21:16:55</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>20:22:44</t>
+          <t>21:16:57</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2646,17 +2646,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>20:22:37</t>
+          <t>21:16:53</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>20:22:39</t>
+          <t>21:16:54</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2673,22 +2673,22 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>20:13:03</t>
+          <t>21:16:49</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>20:13:05</t>
+          <t>21:16:50</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2700,22 +2700,22 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>19:49:47</t>
+          <t>21:10:35</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>19:49:48</t>
+          <t>21:10:35</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2727,22 +2727,22 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>19:49:43</t>
+          <t>21:10:15</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>19:49:44</t>
+          <t>21:10:16</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2754,17 +2754,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>19:49:40</t>
+          <t>21:10:14</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>19:49:41</t>
+          <t>21:10:15</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2781,17 +2781,17 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>19:48:23</t>
+          <t>21:10:12</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>19:48:24</t>
+          <t>21:10:13</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2808,17 +2808,17 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>19:47:57</t>
+          <t>21:08:54</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>19:47:58</t>
+          <t>21:08:54</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2835,17 +2835,17 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>19:47:44</t>
+          <t>21:08:51</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>19:47:44</t>
+          <t>21:08:52</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2862,22 +2862,22 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>19:47:42</t>
+          <t>21:08:49</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>19:47:43</t>
+          <t>21:08:51</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2889,22 +2889,22 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>19:43:41</t>
+          <t>21:08:46</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>19:43:42</t>
+          <t>21:08:49</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2916,22 +2916,22 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>19:43:38</t>
+          <t>21:07:20</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>19:43:39</t>
+          <t>21:07:20</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2943,22 +2943,22 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>19:43:08</t>
+          <t>21:07:14</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>19:43:11</t>
+          <t>21:07:15</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>00:00:03</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2970,17 +2970,17 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>19:43:05</t>
+          <t>21:03:01</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>19:43:06</t>
+          <t>21:03:03</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2997,22 +2997,22 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>25/09/2022</t>
+          <t>26/09/2022</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>19:43:02</t>
+          <t>21:02:53</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>19:43:03</t>
+          <t>21:02:56</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:02</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -3024,49 +3024,49 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>21:47:16</t>
+          <t>23:34:10</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>21:47:18</t>
+          <t>23:34:10</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>00:00:34</t>
+          <t>00:00:33</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>21:47:14</t>
+          <t>21:03:18</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>21:47:15</t>
+          <t>21:03:19</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -3078,17 +3078,17 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>21:47:11</t>
+          <t>21:03:14</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>21:47:12</t>
+          <t>21:03:16</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3105,22 +3105,22 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>20:59:48</t>
+          <t>21:03:00</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>20:59:51</t>
+          <t>21:03:00</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -3132,22 +3132,22 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>20:59:44</t>
+          <t>21:02:59</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>20:59:46</t>
+          <t>21:02:59</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -3159,22 +3159,22 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>20:58:43</t>
+          <t>21:02:58</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>20:58:46</t>
+          <t>21:02:59</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -3186,22 +3186,22 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>20:58:39</t>
+          <t>21:02:54</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>20:58:41</t>
+          <t>21:02:56</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3213,17 +3213,17 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>20:58:34</t>
+          <t>21:02:52</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>20:58:36</t>
+          <t>21:02:53</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -3240,22 +3240,22 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>20:53:22</t>
+          <t>21:02:45</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>20:53:23</t>
+          <t>21:02:49</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:03</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -3267,22 +3267,22 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>20:53:21</t>
+          <t>21:02:29</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>20:53:22</t>
+          <t>21:02:34</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>00:00:00</t>
+          <t>00:00:05</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -3294,22 +3294,22 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>20:53:18</t>
+          <t>21:02:21</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>20:53:20</t>
+          <t>21:02:22</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3321,17 +3321,17 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>20:53:15</t>
+          <t>21:02:19</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>20:53:16</t>
+          <t>21:02:20</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -3348,17 +3348,17 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>20:51:14</t>
+          <t>21:02:17</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>20:51:14</t>
+          <t>21:02:18</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -3375,22 +3375,22 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>20:51:08</t>
+          <t>21:00:56</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>20:51:11</t>
+          <t>21:00:57</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -3402,22 +3402,22 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>20:51:05</t>
+          <t>21:00:55</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>20:51:07</t>
+          <t>21:00:56</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -3429,22 +3429,22 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>20:51:02</t>
+          <t>21:00:53</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>20:51:04</t>
+          <t>21:00:54</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -3456,22 +3456,22 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>20:50:52</t>
+          <t>21:00:51</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>20:50:59</t>
+          <t>21:00:52</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -3483,17 +3483,17 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>20:48:59</t>
+          <t>20:56:22</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>20:49:00</t>
+          <t>20:56:24</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -3510,22 +3510,22 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>20:38:47</t>
+          <t>20:56:20</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>20:38:53</t>
+          <t>20:56:21</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>00:00:05</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3537,22 +3537,22 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>20:38:43</t>
+          <t>20:56:18</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>20:38:45</t>
+          <t>20:56:19</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3564,22 +3564,22 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>20:38:41</t>
+          <t>20:45:30</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>20:38:42</t>
+          <t>20:45:31</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -3591,22 +3591,22 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>23/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>20:38:38</t>
+          <t>20:45:02</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>20:38:40</t>
+          <t>20:45:03</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>00:00:02</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -3618,49 +3618,49 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>20:17:31</t>
+          <t>20:40:53</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>20:17:38</t>
+          <t>20:40:54</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>00:00:07</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>01:08:22</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>20:17:26</t>
+          <t>20:40:00</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>20:17:28</t>
+          <t>20:40:01</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>00:00:01</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -3672,22 +3672,22 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>20:12:24</t>
+          <t>20:34:57</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>20:12:29</t>
+          <t>20:34:58</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>00:00:04</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -3699,22 +3699,22 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>20:11:56</t>
+          <t>20:32:57</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>20:12:03</t>
+          <t>20:32:57</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>00:00:06</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -3726,22 +3726,22 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>20:11:27</t>
+          <t>20:32:54</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>20:11:47</t>
+          <t>20:32:55</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>00:00:20</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -3753,22 +3753,22 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>15:16:16</t>
+          <t>20:32:50</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>15:26:35</t>
+          <t>20:32:52</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>00:10:18</t>
+          <t>00:00:01</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -3780,22 +3780,22 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>15:05:33</t>
+          <t>20:31:27</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>15:16:04</t>
+          <t>20:31:28</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>00:10:30</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -3807,22 +3807,22 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>22/09/2022</t>
+          <t>25/09/2022</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>14:18:27</t>
+          <t>20:30:38</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>15:05:20</t>
+          <t>20:30:39</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>00:46:52</t>
+          <t>00:00:00</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -3834,25 +3834,1294 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>20:22:47</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>20:22:50</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>20:22:45</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>20:22:46</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>20:22:43</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>20:22:44</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>20:22:37</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>20:22:39</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>20:13:03</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>20:13:05</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>19:49:47</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>19:49:48</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>19:49:43</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>19:49:44</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>19:49:40</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>19:49:41</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>19:48:23</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>19:48:24</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>19:47:57</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>19:47:58</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>19:47:44</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>19:47:44</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>19:47:42</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>19:47:43</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>19:43:41</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>19:43:42</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>19:43:38</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>19:43:39</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>19:43:08</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>19:43:11</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>00:00:03</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>19:43:05</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>19:43:06</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>25/09/2022</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>19:43:02</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>19:43:03</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>21:47:16</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>21:47:18</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>00:00:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>21:47:14</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>21:47:15</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>21:47:11</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>21:47:12</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>20:59:48</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>20:59:51</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>20:59:44</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>20:59:46</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>20:58:43</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>20:58:46</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>20:58:39</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>20:58:41</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>20:58:34</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>20:58:36</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>20:53:22</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>20:53:23</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>20:53:21</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>20:53:22</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>20:53:18</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>20:53:20</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>20:53:15</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>20:53:16</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>20:51:14</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>20:51:14</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>00:00:00</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>20:51:08</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>20:51:11</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>20:51:05</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>20:51:07</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>20:51:02</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>20:51:04</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>20:50:52</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>20:50:59</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>00:00:06</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>20:48:59</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>20:49:00</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>20:38:47</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>20:38:53</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>00:00:05</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>20:38:43</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>20:38:45</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>20:38:41</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>20:38:42</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>23/09/2022</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>20:38:38</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>20:38:40</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>00:00:02</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
           <t>22/09/2022</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr">
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>20:17:31</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>20:17:38</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>00:00:07</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>01:08:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>20:17:26</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>20:17:28</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>00:00:01</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>20:12:24</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>20:12:29</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>00:00:04</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>20:11:56</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>20:12:03</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>00:00:06</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>20:11:27</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>20:11:47</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>00:00:20</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>15:16:16</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>15:26:35</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>00:10:18</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>15:05:33</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>15:16:04</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>00:10:30</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>14:18:27</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>15:05:20</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>00:46:52</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>22/09/2022</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
         <is>
           <t>14:10:03</t>
         </is>
       </c>
-      <c r="C127" t="inlineStr">
+      <c r="C174" t="inlineStr">
         <is>
           <t>14:10:07</t>
         </is>
       </c>
-      <c r="D127" t="inlineStr">
+      <c r="D174" t="inlineStr">
         <is>
           <t>00:00:04</t>
         </is>
       </c>
-      <c r="E127" t="inlineStr">
+      <c r="E174" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>

</xml_diff>